<commit_message>
created the git ignore file
</commit_message>
<xml_diff>
--- a/data_output/Box_Office1.xlsx
+++ b/data_output/Box_Office1.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,7 +503,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -513,12 +513,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$9,046,059</t>
+          <t>$19,102,299</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-52.6%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -531,16 +531,16 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>$2,603</t>
+          <t>$5,497</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>$34,885,807</t>
+          <t>$19,102,299</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -548,13 +548,13 @@
         </is>
       </c>
       <c r="L2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="b">
         <v>0</v>
       </c>
       <c r="N2" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="3">
@@ -568,12 +568,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Solo Mio</t>
+          <t>Iron Lung</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>$7,001,169</t>
+          <t>$17,800,000</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3052</v>
+        <v>3015</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -591,12 +591,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>$2,293</t>
+          <t>$5,903</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>$7,001,169</t>
+          <t>$17,800,000</t>
         </is>
       </c>
       <c r="J3" t="n">
@@ -604,17 +604,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Angel</t>
+          <t>Markiplier</t>
         </is>
       </c>
       <c r="L3" t="b">
         <v>1</v>
       </c>
       <c r="M3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="4">
@@ -623,58 +623,58 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Iron Lung</t>
+          <t>Melania</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>$6,000,000</t>
+          <t>$7,161,605</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>-66.3%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>2930</v>
+        <v>1778</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-85</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>$2,047</t>
+          <t>$4,027</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>$30,800,000</t>
+          <t>$7,161,605</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Markiplier</t>
+          <t>Amazon MGM Studios</t>
         </is>
       </c>
       <c r="L4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="5">
@@ -683,58 +683,58 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Stray Kids: The dominATE Experience</t>
+          <t>Zootopia 2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>$5,709,394</t>
+          <t>$5,924,315</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+11.8%</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>1724</v>
+        <v>2876</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-54</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>$3,311</t>
+          <t>$2,059</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>$5,709,394</t>
+          <t>$409,081,674</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Bleecker Street Media</t>
+          <t>Walt Disney Studios Motion Pictures</t>
         </is>
       </c>
       <c r="L5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
       </c>
       <c r="N5" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="6">
@@ -743,58 +743,58 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dracula</t>
+          <t>Avatar: Fire and Ash</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>$4,400,264</t>
+          <t>$5,649,878</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-11.8%</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2050</v>
+        <v>2800</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-350</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>$2,146</t>
+          <t>$2,017</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>$4,400,264</t>
+          <t>$386,276,551</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Vertical Entertainment</t>
+          <t>20th Century Studios</t>
         </is>
       </c>
       <c r="L6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" t="b">
         <v>0</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="7">
@@ -803,58 +803,58 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Zootopia 2</t>
+          <t>Shelter</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>$4,004,779</t>
+          <t>$5,531,028</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>-32.4%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>2715</v>
+        <v>2726</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>-161</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>$1,475</t>
+          <t>$2,028</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>$414,511,500</t>
+          <t>$5,531,028</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Walt Disney Studios Motion Pictures</t>
+          <t>Black Bear</t>
         </is>
       </c>
       <c r="L7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" t="b">
         <v>0</v>
       </c>
       <c r="N7" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="8">
@@ -863,26 +863,26 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>The Strangers: Chapter 3</t>
+          <t>Mercy</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>$3,472,554</t>
+          <t>$4,562,937</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-57.8%</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>2565</v>
+        <v>3468</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -891,30 +891,30 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>$1,353</t>
+          <t>$1,315</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>$3,472,554</t>
+          <t>$19,240,756</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Lionsgate</t>
+          <t>Amazon MGM Studios</t>
         </is>
       </c>
       <c r="L8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" t="b">
         <v>0</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="9">
@@ -923,48 +923,48 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Avatar: Fire and Ash</t>
+          <t>The Housemaid</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>$3,471,814</t>
+          <t>$3,454,341</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-38.6%</t>
+          <t>-12.4%</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>2365</v>
+        <v>2603</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>-435</t>
+          <t>-404</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>$1,467</t>
+          <t>$1,327</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>$391,505,664</t>
+          <t>$120,639,938</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>20th Century Studios</t>
+          <t>Lionsgate</t>
         </is>
       </c>
       <c r="L9" t="b">
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="10">
@@ -983,48 +983,48 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Shelter</t>
+          <t>Marty Supreme</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>$2,472,373</t>
+          <t>$2,816,468</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-55.3%</t>
+          <t>-20.6%</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>2726</v>
+        <v>1703</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-318</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>$906</t>
+          <t>$1,653</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>$10,034,168</t>
+          <t>$90,782,571</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Black Bear</t>
+          <t>A24</t>
         </is>
       </c>
       <c r="L10" t="b">
@@ -1034,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="11">
@@ -1043,48 +1043,48 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Melania</t>
+          <t>28 Years Later: The Bone Temple</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>$2,350,783</t>
+          <t>$1,570,165</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>-67.2%</t>
+          <t>-54.2%</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>2003</v>
+        <v>2042</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>+225</t>
+          <t>-1464</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>$1,173</t>
+          <t>$768</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>$13,325,728</t>
+          <t>$23,620,907</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Amazon MGM Studios</t>
+          <t>Sony Pictures Releasing</t>
         </is>
       </c>
       <c r="L11" t="b">
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="12">
@@ -1103,48 +1103,48 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Mercy</t>
+          <t>Hamnet</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>$1,874,459</t>
+          <t>$1,558,355</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>-58.9%</t>
+          <t>-16.1%</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>2502</v>
+        <v>1259</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>-966</t>
+          <t>-737</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>$749</t>
+          <t>$1,237</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>$22,673,749</t>
+          <t>$20,273,385</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Amazon MGM Studios</t>
+          <t>Focus Features</t>
         </is>
       </c>
       <c r="L12" t="b">
@@ -1154,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="13">
@@ -1163,48 +1163,48 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>The Housemaid</t>
+          <t>Return to Silent Hill</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>$1,700,498</t>
+          <t>$980,833</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>-50.8%</t>
+          <t>-69.8%</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>2030</v>
+        <v>1608</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>-573</t>
+          <t>-392</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>$837</t>
+          <t>$609</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>$123,552,778</t>
+          <t>$5,107,032</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Lionsgate</t>
+          <t>Cineverse</t>
         </is>
       </c>
       <c r="L13" t="b">
@@ -1214,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="14">
@@ -1223,48 +1223,48 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>The Moment</t>
+          <t>Anaconda</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>$1,630,399</t>
+          <t>$822,656</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>+281%</t>
+          <t>-37.1%</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>581</v>
+        <v>1052</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>+577</t>
+          <t>-755</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>$2,806</t>
+          <t>$781</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>$2,225,032</t>
+          <t>$63,641,811</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>A24</t>
+          <t>Sony Pictures Releasing</t>
         </is>
       </c>
       <c r="L14" t="b">
@@ -1274,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="15">
@@ -1283,48 +1283,48 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Marty Supreme</t>
+          <t>Primate</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>$1,310,791</t>
+          <t>$814,578</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>-53.5%</t>
+          <t>-47.6%</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>1124</v>
+        <v>1225</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>-579</t>
+          <t>-920</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>$1,166</t>
+          <t>$664</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>$93,217,786</t>
+          <t>$25,075,536</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>A24</t>
+          <t>Paramount Pictures International</t>
         </is>
       </c>
       <c r="L15" t="b">
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="16">
@@ -1343,58 +1343,58 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Hamnet</t>
+          <t>Back to the Past</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>$771,560</t>
+          <t>$694,790</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>-50.5%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>925</v>
+        <v>64</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>-334</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>$834</t>
+          <t>$10,856</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>$21,786,265</t>
+          <t>$694,790</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Focus Features</t>
+          <t>Well Go USA Entertainment</t>
         </is>
       </c>
       <c r="L16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" t="b">
         <v>0</v>
       </c>
       <c r="N16" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="17">
@@ -1403,58 +1403,58 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Whistle</t>
+          <t>The SpongeBob Movie: Search for SquarePants</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>$705,080</t>
+          <t>$606,038</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-32.9%</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>1200</v>
+        <v>802</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-614</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>$587</t>
+          <t>$755</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>$705,080</t>
+          <t>$70,540,996</t>
         </is>
       </c>
       <c r="J17" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>IFC Films</t>
+          <t>Paramount Pictures International</t>
         </is>
       </c>
       <c r="L17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" t="b">
         <v>0</v>
       </c>
       <c r="N17" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="18">
@@ -1463,48 +1463,48 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>28 Years Later: The Bone Temple</t>
+          <t>Song Sung Blue</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>$474,595</t>
+          <t>$583,180</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>-69.8%</t>
+          <t>-24.1%</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>785</v>
+        <v>709</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>-1257</t>
+          <t>-443</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>$604</t>
+          <t>$822</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>$24,780,824</t>
+          <t>$38,298,910</t>
         </is>
       </c>
       <c r="J18" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sony Pictures Releasing</t>
+          <t>Focus Features</t>
         </is>
       </c>
       <c r="L18" t="b">
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="19">
@@ -1523,58 +1523,58 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Bendito Corazon</t>
+          <t>Clika</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>$404,000</t>
+          <t>$525,724</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-58.3%</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>23</v>
+        <v>540</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+18</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>$17,565</t>
+          <t>$973</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>$404,000</t>
+          <t>$2,208,179</t>
         </is>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>CNMG Distribución</t>
+          <t>Columbia Pictures</t>
         </is>
       </c>
       <c r="L19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="20">
@@ -1583,58 +1583,58 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Back to the Past</t>
+          <t>The Moment</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>$329,070</t>
+          <t>$427,960</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>-52.6%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>+60</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>$2,653</t>
+          <t>$106,990</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>$1,390,271</t>
+          <t>$427,960</t>
         </is>
       </c>
       <c r="J20" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Well Go USA Entertainment</t>
+          <t>A24</t>
         </is>
       </c>
       <c r="L20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" t="b">
         <v>0</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="21">
@@ -1643,48 +1643,48 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Anaconda</t>
+          <t>No Other Choice</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>$315,752</t>
+          <t>$412,042</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>-61.6%</t>
+          <t>-37.5%</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>545</v>
+        <v>323</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>-507</t>
+          <t>-359</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>$579</t>
+          <t>$1,275</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>$64,218,364</t>
+          <t>$9,105,646</t>
         </is>
       </c>
       <c r="J21" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Sony Pictures Releasing</t>
+          <t>Neon</t>
         </is>
       </c>
       <c r="L21" t="b">
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="22">
@@ -1703,48 +1703,48 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>36</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>The SpongeBob Movie: Search for SquarePants</t>
+          <t>Arco2026 Re-release</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>$242,510</t>
+          <t>$402,554</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>-60%</t>
+          <t>+788.6%</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>453</v>
+        <v>302</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>-349</t>
+          <t>+298</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>$535</t>
+          <t>$1,332</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>$70,919,960</t>
+          <t>$507,768</t>
         </is>
       </c>
       <c r="J22" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Paramount Pictures International</t>
+          <t>Neon</t>
         </is>
       </c>
       <c r="L22" t="b">
@@ -1754,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="23">
@@ -1763,58 +1763,58 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>32</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Pillion</t>
+          <t>A Private Life</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>$241,769</t>
+          <t>$343,410</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+385%</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>4</v>
+        <v>420</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+401</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>$60,442</t>
+          <t>$817</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>$241,769</t>
+          <t>$555,539</t>
         </is>
       </c>
       <c r="J23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>A24</t>
+          <t>Sony Pictures Classics</t>
         </is>
       </c>
       <c r="L23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" t="b">
         <v>0</v>
       </c>
       <c r="N23" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="24">
@@ -1823,40 +1823,40 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Song Sung Blue</t>
+          <t>David</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>$225,675</t>
+          <t>$331,629</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>-61.3%</t>
+          <t>-41.4%</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>448</v>
+        <v>535</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>-261</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>$503</t>
+          <t>$619</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>$38,869,840</t>
+          <t>$79,964,303</t>
         </is>
       </c>
       <c r="J24" t="n">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Focus Features</t>
+          <t>Angel</t>
         </is>
       </c>
       <c r="L24" t="b">
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="N24" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="25">
@@ -1883,26 +1883,26 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Aida: The Movie</t>
+          <t>The Testament of Ann Lee</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>$217,000</t>
+          <t>$317,587</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-43.1%</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>27</v>
+        <v>500</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1911,30 +1911,30 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>$8,037</t>
+          <t>$635</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>$217,000</t>
+          <t>$2,110,097</t>
         </is>
       </c>
       <c r="J25" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Sony Pictures Releasing</t>
+          <t>Searchlight Pictures</t>
         </is>
       </c>
       <c r="L25" t="b">
         <v>0</v>
       </c>
       <c r="M25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="26">
@@ -1943,48 +1943,48 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Scarlet</t>
+          <t>Greenland 2: Migration</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>$212,256</t>
+          <t>$290,394</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-70.2%</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>160</v>
+        <v>614</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-1275</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>$1,326</t>
+          <t>$472</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>$212,256</t>
+          <t>$17,669,539</t>
         </is>
       </c>
       <c r="J26" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Sony Pictures Releasing</t>
+          <t>Lionsgate</t>
         </is>
       </c>
       <c r="L26" t="b">
@@ -1994,7 +1994,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="27">
@@ -2003,44 +2003,44 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>22</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>No Other Choice</t>
+          <t>The Secret Agent</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>$206,916</t>
+          <t>$263,648</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>-49.8%</t>
+          <t>+30%</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>196</v>
+        <v>312</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>-127</t>
+          <t>+167</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>$1,055</t>
+          <t>$845</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>$9,500,807</t>
+          <t>$3,236,628</t>
         </is>
       </c>
       <c r="J27" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="N27" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="28">
@@ -2063,58 +2063,58 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Primate</t>
+          <t>Infinite Icon: A Visual Memoir</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>$192,359</t>
+          <t>$200,000</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>-76.4%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>372</v>
+        <v>677</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>-853</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>$517</t>
+          <t>$295</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>$25,556,289</t>
+          <t>$200,000</t>
         </is>
       </c>
       <c r="J28" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Paramount Pictures International</t>
+          <t>CJ 4DPlex</t>
         </is>
       </c>
       <c r="L28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="29">
@@ -2123,48 +2123,48 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>21</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>The Secret Agent</t>
+          <t>Charlie the Wonderdog</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>$176,626</t>
+          <t>$179,176</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>-33%</t>
+          <t>-47%</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>300</v>
+        <v>625</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>-12</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>$588</t>
+          <t>$286</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>$3,555,262</t>
+          <t>$1,853,217</t>
         </is>
       </c>
       <c r="J29" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Neon</t>
+          <t>Viva Pictures</t>
         </is>
       </c>
       <c r="L29" t="b">
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="N29" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="30">
@@ -2183,48 +2183,48 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>A Private Life</t>
+          <t>Sentimental Value</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>$153,273</t>
+          <t>$149,099</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>-55.4%</t>
+          <t>-26.2%</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>142</v>
+        <v>276</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>-278</t>
+          <t>+169</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>$1,079</t>
+          <t>$540</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>$898,202</t>
+          <t>$4,715,164</t>
         </is>
       </c>
       <c r="J30" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sony Pictures Classics</t>
+          <t>Neon</t>
         </is>
       </c>
       <c r="L30" t="b">
@@ -2234,7 +2234,7 @@
         <v>0</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="31">
@@ -2243,58 +2243,58 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>34</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Clika</t>
+          <t>The Voice of Hind Rajab</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>$140,373</t>
+          <t>$125,717</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>-73.3%</t>
+          <t>+141.7%</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>202</v>
+        <v>108</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>-338</t>
+          <t>+70</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>$694</t>
+          <t>$1,164</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>$2,517,947</t>
+          <t>$598,132</t>
         </is>
       </c>
       <c r="J31" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Columbia Pictures</t>
+          <t>WILLA</t>
         </is>
       </c>
       <c r="L31" t="b">
         <v>0</v>
       </c>
       <c r="M31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="32">
@@ -2303,58 +2303,58 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Sirat2026 Re-release</t>
+          <t>One Battle After Another</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>$137,997</t>
+          <t>$80,088</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-60%</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>4</v>
+        <v>300</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-575</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>$34,499</t>
+          <t>$266</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>$137,997</t>
+          <t>$72,047,339</t>
         </is>
       </c>
       <c r="J32" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Neon</t>
+          <t>Warner Bros.</t>
         </is>
       </c>
       <c r="L32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" t="b">
         <v>0</v>
       </c>
       <c r="N32" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="33">
@@ -2363,48 +2363,48 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>26</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Arco2026 Re-release</t>
+          <t>Standout: The Ben Kjar Story</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>$136,103</t>
+          <t>$79,014</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>-66.2%</t>
+          <t>-47.7%</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>243</v>
+        <v>52</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>-59</t>
+          <t>-40</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>$560</t>
+          <t>$1,519</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>$812,427</t>
+          <t>$308,161</t>
         </is>
       </c>
       <c r="J33" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Neon</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L33" t="b">
@@ -2414,7 +2414,7 @@
         <v>0</v>
       </c>
       <c r="N33" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="34">
@@ -2423,58 +2423,58 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>35</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Return to Silent Hill</t>
+          <t>All That's Left of You</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>$115,559</t>
+          <t>$50,217</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>-88.2%</t>
+          <t>+0.7%</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>273</v>
+        <v>43</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>-1335</t>
+          <t>-9</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>$423</t>
+          <t>$1,167</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>$5,544,971</t>
+          <t>$350,228</t>
         </is>
       </c>
       <c r="J34" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Cineverse</t>
+          <t>Watermelon Pictures</t>
         </is>
       </c>
       <c r="L34" t="b">
         <v>0</v>
       </c>
       <c r="M34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="35">
@@ -2483,48 +2483,48 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>33</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>The Choral</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>$109,248</t>
+          <t>$47,909</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>-67.1%</t>
+          <t>-30.1%</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>256</v>
+        <v>51</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>-279</t>
+          <t>-63</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>$426</t>
+          <t>$939</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>$80,207,361</t>
+          <t>$791,014</t>
         </is>
       </c>
       <c r="J35" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Angel</t>
+          <t>Sony Pictures Classics</t>
         </is>
       </c>
       <c r="L35" t="b">
@@ -2534,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="N35" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="36">
@@ -2543,40 +2543,40 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>28</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>The Testament of Ann Lee</t>
+          <t>Is This Thing On?</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>$106,490</t>
+          <t>$44,109</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>-66.5%</t>
+          <t>-70.5%</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>230</v>
+        <v>95</v>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>-270</t>
+          <t>-205</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>$463</t>
+          <t>$464</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>$2,380,323</t>
+          <t>$6,140,680</t>
         </is>
       </c>
       <c r="J36" t="n">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Searchlight Pictures</t>
+          <t>Walt Disney Studios Motion Pictures</t>
         </is>
       </c>
       <c r="L36" t="b">
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
       <c r="N36" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="37">
@@ -2603,58 +2603,58 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Sentimental Value</t>
+          <t>A Poet</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>$78,897</t>
+          <t>$27,754</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>-47.1%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>251</v>
+        <v>2</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>-25</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>$314</t>
+          <t>$13,877</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>$4,870,951</t>
+          <t>$27,754</t>
         </is>
       </c>
       <c r="J37" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Neon</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M37" t="b">
         <v>0</v>
       </c>
       <c r="N37" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="38">
@@ -2663,26 +2663,26 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Charlie the Wonderdog</t>
+          <t>Islands</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>$70,068</t>
+          <t>$26,717</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>-60.9%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>625</v>
+        <v>44</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
@@ -2691,30 +2691,30 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>$112</t>
+          <t>$607</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>$1,946,963</t>
+          <t>$26,717</t>
         </is>
       </c>
       <c r="J38" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Viva Pictures</t>
+          <t>Greenwich Entertainment</t>
         </is>
       </c>
       <c r="L38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" t="b">
         <v>0</v>
       </c>
       <c r="N38" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="39">
@@ -2723,58 +2723,58 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>29</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>The Voice of Hind Rajab</t>
+          <t>H Is for Hawk</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>$66,175</t>
+          <t>$23,972</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>-47.4%</t>
+          <t>-83.7%</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>+12</t>
+          <t>-380</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>$551</t>
+          <t>$249</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>$738,478</t>
+          <t>$275,705</t>
         </is>
       </c>
       <c r="J39" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>WILLA</t>
+          <t>Roadside Attractions</t>
         </is>
       </c>
       <c r="L39" t="b">
         <v>0</v>
       </c>
       <c r="M39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N39" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="40">
@@ -2783,58 +2783,58 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>A Poet</t>
+          <t>The Love That Remains</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>$51,808</t>
+          <t>$23,248</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>+86.7%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>+31</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>$1,569</t>
+          <t>$11,624</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>$91,441</t>
+          <t>$23,248</t>
         </is>
       </c>
       <c r="J40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Janus Films</t>
         </is>
       </c>
       <c r="L40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M40" t="b">
         <v>0</v>
       </c>
       <c r="N40" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="41">
@@ -2843,48 +2843,48 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>40</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Standout: The Ben Kjar Story</t>
+          <t>Father Mother Sister Brother</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>$48,974</t>
+          <t>$22,603</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>-38%</t>
+          <t>-15.2%</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>-8</t>
+          <t>-14</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>$1,113</t>
+          <t>$869</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>$411,559</t>
+          <t>$917,084</t>
         </is>
       </c>
       <c r="J41" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>MUBI</t>
         </is>
       </c>
       <c r="L41" t="b">
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="N41" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="42">
@@ -2903,48 +2903,48 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>39</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Kokuho</t>
+          <t>Magellan</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>$47,583</t>
+          <t>$20,371</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-26.4%</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-4</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>$15,861</t>
+          <t>$1,273</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>$125,175</t>
+          <t>$143,486</t>
         </is>
       </c>
       <c r="J42" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>GKIDS</t>
+          <t>Janus Films</t>
         </is>
       </c>
       <c r="L42" t="b">
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="N42" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="43">
@@ -2963,58 +2963,58 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>One Battle After Another</t>
+          <t>Natchez</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>$47,434</t>
+          <t>$17,016</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>-40.8%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>230</v>
+        <v>1</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>-70</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>$206</t>
+          <t>$17,016</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>$72,127,739</t>
+          <t>$29,041</t>
         </is>
       </c>
       <c r="J43" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Warner Bros.</t>
+          <t>Oscilloscope</t>
         </is>
       </c>
       <c r="L43" t="b">
         <v>0</v>
       </c>
       <c r="M43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N43" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="44">
@@ -3023,58 +3023,58 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>45</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>All That's Left of You</t>
+          <t>Sound of Falling</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>$37,024</t>
+          <t>$14,318</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>-26.3%</t>
+          <t>+15.1%</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>-10</t>
+          <t>+16</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>$1,121</t>
+          <t>$681</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>$413,913</t>
+          <t>$53,903</t>
         </is>
       </c>
       <c r="J44" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Watermelon Pictures</t>
+          <t>MUBI</t>
         </is>
       </c>
       <c r="L44" t="b">
         <v>0</v>
       </c>
       <c r="M44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="45">
@@ -3083,58 +3083,58 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>58</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Buffalo Kids</t>
+          <t>Angel's Egg</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>$36,681</t>
+          <t>$13,489</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+667.7%</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>750</v>
+        <v>2</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-2</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>$48</t>
+          <t>$6,744</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>$111,577</t>
+          <t>$862,717</t>
         </is>
       </c>
       <c r="J45" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Viva Pictures</t>
+          <t>GKIDS</t>
         </is>
       </c>
       <c r="L45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="46">
@@ -3143,58 +3143,58 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>25</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>The Choral</t>
+          <t>Dead Man's Wire</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>$30,147</t>
+          <t>$12,980</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>-37.1%</t>
+          <t>-92.2%</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>-10</t>
+          <t>-586</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>$735</t>
+          <t>$370</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>$858,178</t>
+          <t>$2,223,703</t>
         </is>
       </c>
       <c r="J46" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sony Pictures Classics</t>
+          <t>Row K Entertainment</t>
         </is>
       </c>
       <c r="L46" t="b">
         <v>0</v>
       </c>
       <c r="M46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N46" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="47">
@@ -3203,44 +3203,44 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>37</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Magellan</t>
+          <t>Resurrection</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>$21,938</t>
+          <t>$11,552</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>+7.7%</t>
+          <t>-61.9%</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>+7</t>
+          <t>-11</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>$953</t>
+          <t>$608</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>$175,089</t>
+          <t>$582,900</t>
         </is>
       </c>
       <c r="J47" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -3254,7 +3254,7 @@
         <v>0</v>
       </c>
       <c r="N47" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="48">
@@ -3263,48 +3263,48 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>57</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Is This Thing On?</t>
+          <t>Fuck My Son!</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>$19,093</t>
+          <t>$10,498</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>-56.7%</t>
+          <t>+467.2%</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>-20</t>
+          <t>+21</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>$254</t>
+          <t>$437</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>$6,176,849</t>
+          <t>$55,426</t>
         </is>
       </c>
       <c r="J48" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Walt Disney Studios Motion Pictures</t>
+          <t>Cartuna</t>
         </is>
       </c>
       <c r="L48" t="b">
@@ -3314,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="N48" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="49">
@@ -3323,48 +3323,48 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>47</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>The Love That Remains</t>
+          <t>Blue Moon</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>$14,840</t>
+          <t>$9,378</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>-36.2%</t>
+          <t>-6.3%</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>+6</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>$1,855</t>
+          <t>$375</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>$46,380</t>
+          <t>$2,122,607</t>
         </is>
       </c>
       <c r="J49" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Janus Films</t>
+          <t>Sony Pictures Classics</t>
         </is>
       </c>
       <c r="L49" t="b">
@@ -3374,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="N49" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="50">
@@ -3383,48 +3383,48 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>30</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Mr. Nobody Against Putin</t>
+          <t>Hard Boiled2026 Re-release</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>$11,018</t>
+          <t>$8,707</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>+193.4%</t>
+          <t>-93.7%</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>+16</t>
+          <t>-500</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>$550</t>
+          <t>$72</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>$35,941</t>
+          <t>$382,686</t>
         </is>
       </c>
       <c r="J50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Kino Lorber</t>
+          <t>GKIDS</t>
         </is>
       </c>
       <c r="L50" t="b">
@@ -3434,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="N50" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="51">
@@ -3443,44 +3443,44 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>52</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>The President's Cake</t>
+          <t>Nuremberg</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>$9,919</t>
+          <t>$6,194</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+8.5%</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-13</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>$3,306</t>
+          <t>$516</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>$9,919</t>
+          <t>$14,515,847</t>
         </is>
       </c>
       <c r="J51" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -3488,13 +3488,13 @@
         </is>
       </c>
       <c r="L51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51" t="b">
         <v>0</v>
       </c>
       <c r="N51" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="52">
@@ -3503,40 +3503,40 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>62</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Sound of Falling</t>
+          <t>Holding Liat</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>$8,857</t>
+          <t>$4,763</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>-38.1%</t>
+          <t>+295.6%</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>+1</t>
+          <t>-2</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>$402</t>
+          <t>$2,381</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>$72,557</t>
+          <t>$33,530</t>
         </is>
       </c>
       <c r="J52" t="n">
@@ -3544,7 +3544,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>MUBI</t>
+          <t>The Film Collaborative</t>
         </is>
       </c>
       <c r="L52" t="b">
@@ -3554,7 +3554,7 @@
         <v>0</v>
       </c>
       <c r="N52" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="53">
@@ -3563,48 +3563,48 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>44</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Resurrection</t>
+          <t>We Bury the Dead</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>$8,743</t>
+          <t>$4,191</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>-24.3%</t>
+          <t>-67%</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>-6</t>
+          <t>-7</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>$672</t>
+          <t>$523</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>$595,679</t>
+          <t>$3,711,110</t>
         </is>
       </c>
       <c r="J53" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Janus Films</t>
+          <t>Vertical Entertainment</t>
         </is>
       </c>
       <c r="L53" t="b">
@@ -3614,7 +3614,7 @@
         <v>0</v>
       </c>
       <c r="N53" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="54">
@@ -3623,58 +3623,58 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Natchez</t>
+          <t>Paying for It</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>$8,474</t>
+          <t>$4,060</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>-50.2%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>+2</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>$2,824</t>
+          <t>$4,060</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>$46,577</t>
+          <t>$7,917</t>
         </is>
       </c>
       <c r="J54" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Oscilloscope</t>
+          <t>Film Movement</t>
         </is>
       </c>
       <c r="L54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N54" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="55">
@@ -3683,48 +3683,48 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>38</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Blue Moon</t>
+          <t>Atropia</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>$8,295</t>
+          <t>$3,896</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>-11.5%</t>
+          <t>-86.5%</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>-8</t>
+          <t>-9</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>$487</t>
+          <t>$243</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>$2,140,796</t>
+          <t>$61,416</t>
         </is>
       </c>
       <c r="J55" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Sony Pictures Classics</t>
+          <t>Vertical Entertainment</t>
         </is>
       </c>
       <c r="L55" t="b">
@@ -3734,7 +3734,7 @@
         <v>0</v>
       </c>
       <c r="N55" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="56">
@@ -3743,48 +3743,48 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Holding Liat</t>
+          <t>Mr. Nobody Against Putin</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>$7,260</t>
+          <t>$3,755</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>+52.4%</t>
+          <t>-15.9%</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>+1</t>
+          <t>+3</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>$2,420</t>
+          <t>$938</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>$41,224</t>
+          <t>$19,376</t>
         </is>
       </c>
       <c r="J56" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>The Film Collaborative</t>
+          <t>Kino Lorber</t>
         </is>
       </c>
       <c r="L56" t="b">
@@ -3794,7 +3794,7 @@
         <v>0</v>
       </c>
       <c r="N56" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="57">
@@ -3803,54 +3803,58 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>51</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>The Librarians</t>
+          <t>Obex</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>$6,965</t>
+          <t>$3,697</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-42.7%</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-2</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>$3,482</t>
+          <t>$410</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>$288,354</t>
+          <t>$40,078</t>
         </is>
       </c>
       <c r="J57" t="n">
-        <v>19</v>
-      </c>
-      <c r="K57" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Oscilloscope</t>
+        </is>
+      </c>
       <c r="L57" t="b">
         <v>0</v>
       </c>
       <c r="M57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N57" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="58">
@@ -3859,26 +3863,26 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>55</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Dead Man's Wire</t>
+          <t>Conversation Piece2025 Re-release</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>$6,736</t>
+          <t>$2,253</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>-48.1%</t>
+          <t>-36.9%</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
@@ -3887,30 +3891,30 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>$192</t>
+          <t>$2,253</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>$2,236,813</t>
+          <t>$10,285</t>
         </is>
       </c>
       <c r="J58" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>Row K Entertainment</t>
+          <t>Kino Lorber</t>
         </is>
       </c>
       <c r="L58" t="b">
         <v>0</v>
       </c>
       <c r="M58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N58" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="59">
@@ -3919,48 +3923,48 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>41</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Father Mother Sister Brother</t>
+          <t>All You Need Is Kill</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>$6,583</t>
+          <t>$1,651</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>-70.9%</t>
+          <t>-92.7%</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>-12</t>
+          <t>-75</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>$470</t>
+          <t>$412</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>$934,415</t>
+          <t>$691,789</t>
         </is>
       </c>
       <c r="J59" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>MUBI</t>
+          <t>GKIDS</t>
         </is>
       </c>
       <c r="L59" t="b">
@@ -3970,7 +3974,7 @@
         <v>0</v>
       </c>
       <c r="N59" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="60">
@@ -3979,58 +3983,58 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>46</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Jimpa</t>
+          <t>Rosemead</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>$6,395</t>
+          <t>$1,234</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-88.3%</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-6</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>$913</t>
+          <t>$617</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>$18,109</t>
+          <t>$287,217</t>
         </is>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>Kino Lorber</t>
+          <t>Vertical Entertainment</t>
         </is>
       </c>
       <c r="L60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M60" t="b">
         <v>0</v>
       </c>
       <c r="N60" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="61">
@@ -4039,48 +4043,48 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>63</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>H Is for Hawk</t>
+          <t>Hundreds of Beavers</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>$5,864</t>
+          <t>$1,225</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>-75.5%</t>
+          <t>+34.6%</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>-76</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>$293</t>
+          <t>$1,225</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>$298,570</t>
+          <t>$868,639</t>
         </is>
       </c>
       <c r="J61" t="n">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Roadside Attractions</t>
+          <t>SRH</t>
         </is>
       </c>
       <c r="L61" t="b">
@@ -4090,7 +4094,7 @@
         <v>0</v>
       </c>
       <c r="N61" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="62">
@@ -4099,58 +4103,58 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>54</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Starman</t>
+          <t>I Was a Stranger</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>$5,355</t>
+          <t>$1,022</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-76.6%</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-30</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>$5,355</t>
+          <t>$102</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>$5,355</t>
+          <t>$2,008,406</t>
         </is>
       </c>
       <c r="J62" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Angel</t>
         </is>
       </c>
       <c r="L62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M62" t="b">
         <v>0</v>
       </c>
       <c r="N62" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="63">
@@ -4159,48 +4163,48 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>60</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Islands</t>
+          <t>Put Your Soul on Your Hand and Walk</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>$3,833</t>
+          <t>$929</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>-85.7%</t>
+          <t>-35%</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>-29</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>$255</t>
+          <t>$929</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>$46,130</t>
+          <t>$50,133</t>
         </is>
       </c>
       <c r="J63" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Greenwich Entertainment</t>
+          <t>Kino Lorber</t>
         </is>
       </c>
       <c r="L63" t="b">
@@ -4210,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="N63" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="64">
@@ -4219,58 +4223,58 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Obex</t>
+          <t>Killer of Sheep2025 Re-release</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>$3,442</t>
+          <t>$714</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>-6.9%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>-4</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>$688</t>
+          <t>$714</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>$45,207</t>
+          <t>$101,895</t>
         </is>
       </c>
       <c r="J64" t="n">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>Oscilloscope</t>
+          <t>Kino Lorber</t>
         </is>
       </c>
       <c r="L64" t="b">
         <v>0</v>
       </c>
       <c r="M64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N64" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="65">
@@ -4279,22 +4283,22 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>56</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Conversation Piece2025 Re-release</t>
+          <t>Queen Kelly</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>$1,915</t>
+          <t>$648</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>-15%</t>
+          <t>-79.3%</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -4302,17 +4306,17 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>+1</t>
+          <t>-4</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>$957</t>
+          <t>$324</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>$14,685</t>
+          <t>$22,282</t>
         </is>
       </c>
       <c r="J65" t="n">
@@ -4330,7 +4334,7 @@
         <v>0</v>
       </c>
       <c r="N65" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="66">
@@ -4339,22 +4343,22 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>68</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Ain't No Back to a Merry-Go-Round</t>
+          <t>Seeds</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>$1,448</t>
+          <t>$575</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+53.3%</t>
         </is>
       </c>
       <c r="F66" t="n">
@@ -4367,20 +4371,20 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>$1,448</t>
+          <t>$575</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>$76,793</t>
+          <t>$34,175</t>
         </is>
       </c>
       <c r="J66" t="n">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Indican Pictures</t>
         </is>
       </c>
       <c r="L66" t="b">
@@ -4390,7 +4394,7 @@
         <v>0</v>
       </c>
       <c r="N66" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="67">
@@ -4399,48 +4403,48 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>65</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Paying for It</t>
+          <t>Killer Raccoons! 2! Dark Christmas in the Dark!2025 Re-release</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>$1,240</t>
+          <t>$250</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>-69.5%</t>
+          <t>-44.4%</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>+2</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>$413</t>
+          <t>$250</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>$11,911</t>
+          <t>$17,738</t>
         </is>
       </c>
       <c r="J67" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Film Movement</t>
+          <t>Indican Pictures</t>
         </is>
       </c>
       <c r="L67" t="b">
@@ -4450,7 +4454,7 @@
         <v>0</v>
       </c>
       <c r="N67" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="68">
@@ -4459,22 +4463,22 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Queen Kelly</t>
+          <t>Dust Bunny</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>$1,196</t>
+          <t>$200</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>+84.6%</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F68" t="n">
@@ -4487,20 +4491,20 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>$398</t>
+          <t>$66</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>$23,477</t>
+          <t>$584,724</t>
         </is>
       </c>
       <c r="J68" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Kino Lorber</t>
+          <t>Roadside Attractions</t>
         </is>
       </c>
       <c r="L68" t="b">
@@ -4510,7 +4514,7 @@
         <v>0</v>
       </c>
       <c r="N68" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="69">
@@ -4524,12 +4528,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Can't Let It Go</t>
+          <t>Suspended Time</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>$875</t>
+          <t>$191</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -4547,18 +4551,22 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>$875</t>
+          <t>$191</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>$18,190</t>
+          <t>$19,848</t>
         </is>
       </c>
       <c r="J69" t="n">
-        <v>28</v>
-      </c>
-      <c r="K69" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Music Box Films</t>
+        </is>
+      </c>
       <c r="L69" t="b">
         <v>0</v>
       </c>
@@ -4566,7 +4574,7 @@
         <v>0</v>
       </c>
       <c r="N69" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="70">
@@ -4575,58 +4583,58 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>71</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Killer of Sheep2025 Re-release</t>
+          <t>Mistress Dispeller</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>$787</t>
+          <t>$176</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>+10.2%</t>
+          <t>+76%</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>+1</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>$393</t>
+          <t>$176</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>$102,683</t>
+          <t>$93,248</t>
         </is>
       </c>
       <c r="J70" t="n">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Kino Lorber</t>
+          <t>Oscilloscope</t>
         </is>
       </c>
       <c r="L70" t="b">
         <v>0</v>
       </c>
       <c r="M70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N70" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
     <row r="71">
@@ -4635,22 +4643,22 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>69</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>The Business of Fancydancing2025 Re-release</t>
+          <t>Young Mothers</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>$714</t>
+          <t>$93</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-69.2%</t>
         </is>
       </c>
       <c r="F71" t="n">
@@ -4658,25 +4666,25 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>-1</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>$714</t>
+          <t>$93</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>$7,625</t>
+          <t>$11,291</t>
         </is>
       </c>
       <c r="J71" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Kino Lorber</t>
+          <t>Music Box Films</t>
         </is>
       </c>
       <c r="L71" t="b">
@@ -4686,187 +4694,7 @@
         <v>0</v>
       </c>
       <c r="N71" s="1" t="n">
-        <v>46067.05851589981</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>71</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Put Your Soul on Your Hand and Walk</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>$714</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>-23.1%</t>
-        </is>
-      </c>
-      <c r="F72" t="n">
-        <v>1</v>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>$714</t>
-        </is>
-      </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>$50,848</t>
-        </is>
-      </c>
-      <c r="J72" t="n">
-        <v>14</v>
-      </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>Kino Lorber</t>
-        </is>
-      </c>
-      <c r="L72" t="b">
-        <v>0</v>
-      </c>
-      <c r="M72" t="b">
-        <v>0</v>
-      </c>
-      <c r="N72" s="1" t="n">
-        <v>46067.05851589981</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>72</v>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Seeds</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>$500</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>-13%</t>
-        </is>
-      </c>
-      <c r="F73" t="n">
-        <v>1</v>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>$500</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>$34,800</t>
-        </is>
-      </c>
-      <c r="J73" t="n">
-        <v>25</v>
-      </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>Indican Pictures</t>
-        </is>
-      </c>
-      <c r="L73" t="b">
-        <v>0</v>
-      </c>
-      <c r="M73" t="b">
-        <v>0</v>
-      </c>
-      <c r="N73" s="1" t="n">
-        <v>46067.05851589981</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>73</v>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Fuck My Son!</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>$485</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>-95.4%</t>
-        </is>
-      </c>
-      <c r="F74" t="n">
-        <v>1</v>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>-23</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>$485</t>
-        </is>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>$56,092</t>
-        </is>
-      </c>
-      <c r="J74" t="n">
-        <v>17</v>
-      </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>Cartuna</t>
-        </is>
-      </c>
-      <c r="L74" t="b">
-        <v>0</v>
-      </c>
-      <c r="M74" t="b">
-        <v>0</v>
-      </c>
-      <c r="N74" s="1" t="n">
-        <v>46067.05851589981</v>
+        <v>46067.35578773871</v>
       </c>
     </row>
   </sheetData>

</xml_diff>